<commit_message>
char matched accel implementation only
</commit_message>
<xml_diff>
--- a/accel_final_approach_3class_all.xlsx
+++ b/accel_final_approach_3class_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,13 +463,64 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9600523903077931</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.9590643274853801</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
         <v>9</v>
       </c>
-      <c r="E2" t="n">
-        <v>1</v>
+      <c r="E4" t="n">
+        <v>0.9393939393939394</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9691482226693494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>